<commit_message>
mise à jour xlsx
</commit_message>
<xml_diff>
--- a/audit-SEO.xlsx
+++ b/audit-SEO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>Catégorie</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Même apparence pour les  boutons</t>
   </si>
   <si>
-    <t>Cours OC</t>
-  </si>
-  <si>
     <t>https://www.seo.fr/definition/black-hat-seo  et cours oc</t>
   </si>
   <si>
@@ -173,6 +170,21 @@
   </si>
   <si>
     <t>https://www.solocal.com/ressources/articles/importance-seo-local-strategie-web-to-store</t>
+  </si>
+  <si>
+    <t>https://semji.com/fr/blog/quel-est-linteret-des-balises-h1-h2-h3-pour-votre-seo/</t>
+  </si>
+  <si>
+    <t>https://www.yoma-web.com/conseils-referencement/webdesign/accessibilite-couleur-contraste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réglage des contrastes </t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/guidelines/google-images?hl=fr</t>
+  </si>
+  <si>
+    <t>https://fr.oncrawl.com/seo-technique/accessibilite-web-seo/</t>
   </si>
 </sst>
 </file>
@@ -353,9 +365,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -367,6 +376,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -589,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="44" zoomScaleNormal="63" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="57.6" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -599,51 +611,51 @@
     <col min="2" max="2" width="88.36328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="55.90625" style="2" customWidth="1"/>
     <col min="4" max="4" width="67.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.81640625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="47.81640625" style="19" customWidth="1"/>
     <col min="6" max="6" width="102.6328125" style="2" customWidth="1"/>
     <col min="7" max="26" width="10.54296875" style="2" customWidth="1"/>
     <col min="27" max="16384" width="11.26953125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="3" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
     </row>
     <row r="2" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -662,7 +674,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.35">
@@ -682,7 +694,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
@@ -722,7 +734,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -742,7 +754,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="85.8" customHeight="1" x14ac:dyDescent="0.35">
@@ -761,11 +773,11 @@
       <c r="E7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="19" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="18" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>27</v>
       </c>
@@ -778,9 +790,11 @@
       <c r="D8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="3" t="s">
-        <v>43</v>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="103.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -799,8 +813,8 @@
       <c r="E9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>43</v>
+      <c r="F9" s="23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="112.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -819,8 +833,8 @@
       <c r="E10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>43</v>
+      <c r="F10" s="23" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -845,8 +859,12 @@
     <hyperlink ref="F3" r:id="rId3"/>
     <hyperlink ref="F5" r:id="rId4"/>
     <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId6"/>
+  <pageSetup orientation="landscape" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>